<commit_message>
- conclusão de cenário- 1. completo o cenário de ID_0001 fazer login bem sucedido. - lista de alterações- 1. Criada uma classe para administrar a configuração padrão do navegador; 2. os métodos da classe WaitActions foram convertidos para retornar um resultado booleano  , além de cada um  ter recebido com a sobrecarga de métodos um método que  recebesse um tempo padrão  de espera.
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44A571B-FDFB-483E-9413-DC2315140379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="dadosDeAcesso" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +24,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>nomeDeUsuário</t>
+  </si>
+  <si>
+    <t>ID_0001</t>
+  </si>
+  <si>
+    <t>André Automatizador</t>
+  </si>
+  <si>
+    <t>automacaoteste</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +359,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Conclusão de cenário - 1. completo o cenário de ID_0002 fazer logout bem sucedido. - lista de alterações - 1. no método de buscar o valor da célula do excel da classe ExcelActions foi colocado  um break  na condição para que não fosse mais feita a execução  do for quando a linha que contém o número do id  fosse encontrada . 2.alterada a forma de organização dos pacotes da camada de test, deletado os pacotes logic, model, step e page;  agora será criado sempre um pacote específico para cada   um tipo  de feature a ser testada, exemplo o pacote login da camada de test que recebeu as classes dos pacotes deletados; 3. na classe RunnerTest foi alterado o ~pela palavra not para ignorar as tags a não serem executadas
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44A571B-FDFB-483E-9413-DC2315140379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF8D1C9-1AF5-49FC-9869-78853E7822C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>id</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>automacaoteste</t>
+  </si>
+  <si>
+    <t>ID_0002</t>
   </si>
 </sst>
 </file>
@@ -360,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,6 +397,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- conclusão de cenário - 1. completo o cenário de ID_0006 enviar uma menssagem bem sucedida na sessão de contato.
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA144D01-0551-4B7A-9FDB-595CB9AB9153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A873A4-5BAD-48CC-A209-98FE3EF48F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dadosDeCadastro" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -60,12 +60,21 @@
   <si>
     <t>ID_0004</t>
   </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>emailparatestesautomacao@gmail.com</t>
+  </si>
+  <si>
+    <t>ID_0006</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +86,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,14 +116,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -204,12 +224,9 @@
             <c:strRef>
               <c:f>dadosDeAcesso!$C$1:$C$2</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>senha</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>automacaoteste</c:v>
+                  <c:v>email</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -220,9 +237,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -486,12 +500,9 @@
             <c:strRef>
               <c:f>dadosDeAcesso!$C$1:$C$2</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>senha</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>automacaoteste</c:v>
+                  <c:v>email</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -502,9 +513,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2114,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D545E6-6286-4A87-A380-ACAF904E063F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,19 +2162,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2174,34 +2183,56 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{8424C5DD-A1AB-44D2-A642-0D59C61BDAA4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- conclusão de cenário - 1. completo o cenário de ID_0007 filtrar categoria por laptop e validar a a apresentação de pelo menos um produto da marca dell
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A873A4-5BAD-48CC-A209-98FE3EF48F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48751101-2D19-42AC-BC2D-2F77EB8DD58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>ID_0006</t>
+  </si>
+  <si>
+    <t>ID_0007</t>
+  </si>
+  <si>
+    <t>sem email</t>
   </si>
 </sst>
 </file>
@@ -2162,10 +2168,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2227,6 +2233,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{8424C5DD-A1AB-44D2-A642-0D59C61BDAA4}"/>

</xml_diff>

<commit_message>
- conclusão de cenário 1. completo o cenário de ID_0008 adicionar um produto no carrinho com sucesso - lista de correção de cenário 1. corrigido o método de validar a apresentação do produto (cenário de ID_0007; 2. corrigido o cenário de ID_0007 que fazia um logout ao selecionar uma categoria ao invés de permanecer logado ao selecionar  um filtro - lista de alterações 1. deletado os métodos da classe WebActions que interagia com uma tabela web
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48751101-2D19-42AC-BC2D-2F77EB8DD58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064FC656-3CFB-4B32-825E-1975827660FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>sem email</t>
+  </si>
+  <si>
+    <t>ID_0008</t>
   </si>
 </sst>
 </file>
@@ -2168,10 +2171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2247,6 +2250,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{8424C5DD-A1AB-44D2-A642-0D59C61BDAA4}"/>

</xml_diff>

<commit_message>
- conclusão  de cenário - 1. completo o cenário de ID_0009 adicionar multiplos produtos no carrinho e validar o preço final
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064FC656-3CFB-4B32-825E-1975827660FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29D4EF6-74C4-4927-93E4-CE8E90EF3E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dadosDeCadastro" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>ID_0008</t>
+  </si>
+  <si>
+    <t>ID_0009</t>
   </si>
 </sst>
 </file>
@@ -2171,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2264,6 +2267,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{8424C5DD-A1AB-44D2-A642-0D59C61BDAA4}"/>

</xml_diff>

<commit_message>
- conclusão de cenário - 1. completo o cenário de ID_0010 deletar um produto do carrinho com sucesso - correção de cenário - 1. corrigido o método do cenário de ID_008 que validava se o produto selecionado foi adicionado no carrinho, mudada a maneira de validar o produto antes estava sendo passado o nome do produto direto no Assert, agora está sendo passado de uma forma dinamica - alterações gerais - 1. removido o // que estava no import e na ação de fechar o driver(classe hooks)
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29D4EF6-74C4-4927-93E4-CE8E90EF3E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CD699-1BD5-452E-B7E5-534C39075132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>ID_0009</t>
+  </si>
+  <si>
+    <t>ID_0010</t>
   </si>
 </sst>
 </file>
@@ -2174,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,6 +2284,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{8424C5DD-A1AB-44D2-A642-0D59C61BDAA4}"/>

</xml_diff>

<commit_message>
- cenário em desenvolvimento - 1. ainda em desenvolvimento o cenário de ID_0011 adicionar 2 produtos no carrinho e depois deletar um e validar o preço final
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CD699-1BD5-452E-B7E5-534C39075132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1CAB81-890F-4ED4-B264-1B0DE8CCEBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>ID_0010</t>
+  </si>
+  <si>
+    <t>ID_0011</t>
   </si>
 </sst>
 </file>
@@ -2177,10 +2180,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,6 +2301,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{8424C5DD-A1AB-44D2-A642-0D59C61BDAA4}"/>

</xml_diff>

<commit_message>
- conclusão de cenário - 1. completo o cenário de ID_0012 finalizar o processo de compra com sucesso.
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/massaDeDados.xlsx
+++ b/src/main/resources/test_data/massaDeDados.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreLuizdaSilva\Documents\curso-BDD-comCucumberEmJava\automacao-demoblaze\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1CAB81-890F-4ED4-B264-1B0DE8CCEBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D043580C-14A0-413D-8C03-775C667864A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dadosDeCadastro" sheetId="2" r:id="rId1"/>
-    <sheet name="dadosDeAcesso" sheetId="1" r:id="rId2"/>
+    <sheet name="dadosPessoaisCompra" sheetId="3" r:id="rId2"/>
+    <sheet name="dadosDeAcesso" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>id</t>
   </si>
@@ -86,6 +87,45 @@
   </si>
   <si>
     <t>ID_0011</t>
+  </si>
+  <si>
+    <t>ID_0012</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>país</t>
+  </si>
+  <si>
+    <t>cidade</t>
+  </si>
+  <si>
+    <t>cartão</t>
+  </si>
+  <si>
+    <t>mês</t>
+  </si>
+  <si>
+    <t>ano</t>
+  </si>
+  <si>
+    <t>André</t>
+  </si>
+  <si>
+    <t>brasil</t>
+  </si>
+  <si>
+    <t>santo andré</t>
+  </si>
+  <si>
+    <t>"1234567898765"</t>
+  </si>
+  <si>
+    <t>"8"</t>
+  </si>
+  <si>
+    <t>"1998"</t>
   </si>
 </sst>
 </file>
@@ -138,10 +178,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2179,11 +2221,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14018-5E45-4229-AD96-11C2E9F0EF68}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,6 +2423,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{8424C5DD-A1AB-44D2-A642-0D59C61BDAA4}"/>

</xml_diff>